<commit_message>
Added functionality to import research data via Excel
In this commit, the ability to import research data using an Excel file has been implemented. Handlers have been added to the admin and teacher api routes to process Excel upload for research data. The application will now read the content of the uploaded Excel file, map it with the expected data format, and store the research data in the database. Also, there's an update in the `Password` module in `dosenServices` to encrypt the password and some adjustment to improve the database query in `penelitianRepository`.
</commit_message>
<xml_diff>
--- a/templates/penelitian_admin_template.xlsx
+++ b/templates/penelitian_admin_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericanthony/Projects/nodejs-fullstack/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBF54F0-C098-7E46-A8A0-634C20D7EFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAE3CC0-44D9-4C4E-92D0-6F791D833154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{BA0B9CE4-5C02-954C-B7EB-646A8C7C3342}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17580" xr2:uid="{BA0B9CE4-5C02-954C-B7EB-646A8C7C3342}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>judul_proposal</t>
-  </si>
-  <si>
     <t>biaya_yang_diajukan</t>
   </si>
   <si>
@@ -84,16 +81,15 @@
   </si>
   <si>
     <t>0309096204</t>
+  </si>
+  <si>
+    <t>judul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-[$Rp-3809]* #,##0.00_-;\-[$Rp-3809]* #,##0.00_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-[$Rp-3809]* #,##0_-;\-[$Rp-3809]* #,##0_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -123,13 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,63 +462,63 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="76.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4">
         <v>133860000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>133860000</v>
       </c>
       <c r="D2">
@@ -533,22 +528,26 @@
         <v>2021</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="H2:J2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>